<commit_message>
Minor additions to fields and subcalc, update docs
</commit_message>
<xml_diff>
--- a/emf/templates/subcalc-footprint-template.xlsx
+++ b/emf/templates/subcalc-footprint-template.xlsx
@@ -50,9 +50,6 @@
     <t>Group</t>
   </si>
   <si>
-    <t>The SubCalc template should be filled out as a flat file with entries in all columns for all rows, then saved as a csv.</t>
-  </si>
-  <si>
     <t>Label identifiying unique footprints. This label won't be plotted.</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t>A flag indicating whether the footprint corresponds to modeled power lines (1 = yes, 0 = no)</t>
+  </si>
+  <si>
+    <t>The SubCalc footprint template should be filled out as a flat file with entries in all columns for all rows, then saved as a csv.</t>
   </si>
 </sst>
 </file>
@@ -970,7 +970,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -981,7 +981,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="3" customFormat="1"/>
@@ -990,7 +990,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="3" customFormat="1">
@@ -998,7 +998,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1022,7 +1022,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2">

</xml_diff>

<commit_message>
split readmes, other tune-ups
</commit_message>
<xml_diff>
--- a/emf/templates/subcalc-footprint-template.xlsx
+++ b/emf/templates/subcalc-footprint-template.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="6" r:id="rId1"/>
-    <sheet name="SubCalc_template" sheetId="1" r:id="rId2"/>
+    <sheet name="subcalc-footprint-template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -59,7 +59,7 @@
     <t>A flag indicating whether the footprint corresponds to modeled power lines (1 = yes, 0 = no)</t>
   </si>
   <si>
-    <t>The SubCalc footprint template should be filled out as a flat file with entries in all columns for all rows, then saved as a csv.</t>
+    <t>The subcalc footprint template should be filled out as a flat file with entries in all columns for all rows. It can be kept in excel format or saved to a csv.</t>
   </si>
 </sst>
 </file>
@@ -969,9 +969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -1059,7 +1057,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>